<commit_message>
little form (to be finished) + some json solution for db
</commit_message>
<xml_diff>
--- a/Schichtplan/Lago/plan.xlsx
+++ b/Schichtplan/Lago/plan.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="47">
   <si>
     <t>Wochentag</t>
   </si>
@@ -142,6 +142,9 @@
     <t>So./Feiertage</t>
   </si>
   <si>
+    <t>Donnerstag</t>
+  </si>
+  <si>
     <t>Sonntag</t>
   </si>
   <si>
@@ -152,9 +155,6 @@
   </si>
   <si>
     <t>Mittwoch</t>
-  </si>
-  <si>
-    <t>Donnerstag</t>
   </si>
 </sst>
 </file>
@@ -835,55 +835,55 @@
         <v>42</v>
       </c>
       <c r="B6" s="2">
-        <v>42247</v>
+        <v>42216</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="B7" s="2">
-        <v>42248</v>
+        <v>42217</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B8" s="2">
-        <v>42249</v>
+        <v>42218</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B9" s="2">
-        <v>42250</v>
+        <v>42219</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B10" s="2">
-        <v>42251</v>
+        <v>42220</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="B11" s="2">
-        <v>42252</v>
+        <v>42221</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B12" s="2">
-        <v>42253</v>
+        <v>42222</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -891,55 +891,55 @@
         <v>42</v>
       </c>
       <c r="B13" s="2">
-        <v>42254</v>
+        <v>42223</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="B14" s="2">
-        <v>42255</v>
+        <v>42224</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B15" s="2">
-        <v>42256</v>
+        <v>42225</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B16" s="2">
-        <v>42257</v>
+        <v>42226</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B17" s="2">
-        <v>42258</v>
+        <v>42227</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="B18" s="2">
-        <v>42259</v>
+        <v>42228</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B19" s="2">
-        <v>42260</v>
+        <v>42229</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -947,55 +947,55 @@
         <v>42</v>
       </c>
       <c r="B20" s="2">
-        <v>42261</v>
+        <v>42230</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="B21" s="2">
-        <v>42262</v>
+        <v>42231</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B22" s="2">
-        <v>42263</v>
+        <v>42232</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B23" s="2">
-        <v>42264</v>
+        <v>42233</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B24" s="2">
-        <v>42265</v>
+        <v>42234</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="B25" s="2">
-        <v>42266</v>
+        <v>42235</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B26" s="2">
-        <v>42267</v>
+        <v>42236</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -1003,55 +1003,55 @@
         <v>42</v>
       </c>
       <c r="B27" s="2">
-        <v>42268</v>
+        <v>42237</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="B28" s="2">
-        <v>42269</v>
+        <v>42238</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B29" s="2">
-        <v>42270</v>
+        <v>42239</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B30" s="2">
-        <v>42271</v>
+        <v>42240</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B31" s="2">
-        <v>42272</v>
+        <v>42241</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="B32" s="2">
-        <v>42273</v>
+        <v>42242</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B33" s="2">
-        <v>42274</v>
+        <v>42243</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -1059,19 +1059,24 @@
         <v>42</v>
       </c>
       <c r="B34" s="2">
-        <v>42275</v>
+        <v>42244</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="B35" s="2">
-        <v>42276</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
+        <v>42245</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B36" s="2">
+        <v>42246</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
handlebars, closes #2 #3
</commit_message>
<xml_diff>
--- a/Schichtplan/Lago/plan.xlsx
+++ b/Schichtplan/Lago/plan.xlsx
@@ -142,6 +142,9 @@
     <t>So./Feiertage</t>
   </si>
   <si>
+    <t>Mittwoch</t>
+  </si>
+  <si>
     <t>Donnerstag</t>
   </si>
   <si>
@@ -152,9 +155,6 @@
   </si>
   <si>
     <t>Dienstag</t>
-  </si>
-  <si>
-    <t>Mittwoch</t>
   </si>
 </sst>
 </file>
@@ -835,31 +835,31 @@
         <v>42</v>
       </c>
       <c r="B6" s="2">
-        <v>42216</v>
+        <v>42194</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="B7" s="2">
-        <v>42217</v>
+        <v>42195</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B8" s="2">
-        <v>42218</v>
+        <v>42196</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B9" s="2">
-        <v>42219</v>
+        <v>42197</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -867,7 +867,7 @@
         <v>44</v>
       </c>
       <c r="B10" s="2">
-        <v>42220</v>
+        <v>42198</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -875,7 +875,7 @@
         <v>45</v>
       </c>
       <c r="B11" s="2">
-        <v>42221</v>
+        <v>42199</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -883,7 +883,7 @@
         <v>46</v>
       </c>
       <c r="B12" s="2">
-        <v>42222</v>
+        <v>42200</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -891,31 +891,31 @@
         <v>42</v>
       </c>
       <c r="B13" s="2">
-        <v>42223</v>
+        <v>42201</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="B14" s="2">
-        <v>42224</v>
+        <v>42202</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B15" s="2">
-        <v>42225</v>
+        <v>42203</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B16" s="2">
-        <v>42226</v>
+        <v>42204</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -923,7 +923,7 @@
         <v>44</v>
       </c>
       <c r="B17" s="2">
-        <v>42227</v>
+        <v>42205</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -931,7 +931,7 @@
         <v>45</v>
       </c>
       <c r="B18" s="2">
-        <v>42228</v>
+        <v>42206</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -939,7 +939,7 @@
         <v>46</v>
       </c>
       <c r="B19" s="2">
-        <v>42229</v>
+        <v>42207</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -947,31 +947,31 @@
         <v>42</v>
       </c>
       <c r="B20" s="2">
-        <v>42230</v>
+        <v>42208</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="B21" s="2">
-        <v>42231</v>
+        <v>42209</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B22" s="2">
-        <v>42232</v>
+        <v>42210</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B23" s="2">
-        <v>42233</v>
+        <v>42211</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -979,7 +979,7 @@
         <v>44</v>
       </c>
       <c r="B24" s="2">
-        <v>42234</v>
+        <v>42212</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -987,7 +987,7 @@
         <v>45</v>
       </c>
       <c r="B25" s="2">
-        <v>42235</v>
+        <v>42213</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -995,7 +995,7 @@
         <v>46</v>
       </c>
       <c r="B26" s="2">
-        <v>42236</v>
+        <v>42214</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -1003,31 +1003,31 @@
         <v>42</v>
       </c>
       <c r="B27" s="2">
-        <v>42237</v>
+        <v>42215</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="B28" s="2">
-        <v>42238</v>
+        <v>42216</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B29" s="2">
-        <v>42239</v>
+        <v>42217</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B30" s="2">
-        <v>42240</v>
+        <v>42218</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -1035,7 +1035,7 @@
         <v>44</v>
       </c>
       <c r="B31" s="2">
-        <v>42241</v>
+        <v>42219</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -1043,7 +1043,7 @@
         <v>45</v>
       </c>
       <c r="B32" s="2">
-        <v>42242</v>
+        <v>42220</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -1051,7 +1051,7 @@
         <v>46</v>
       </c>
       <c r="B33" s="2">
-        <v>42243</v>
+        <v>42221</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -1059,23 +1059,23 @@
         <v>42</v>
       </c>
       <c r="B34" s="2">
-        <v>42244</v>
+        <v>42222</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="B35" s="2">
-        <v>42245</v>
+        <v>42223</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B36" s="2">
-        <v>42246</v>
+        <v>42224</v>
       </c>
     </row>
   </sheetData>

</xml_diff>